<commit_message>
Test data with Icon column
</commit_message>
<xml_diff>
--- a/examples/Team Board for Product Development.xlsx
+++ b/examples/Team Board for Product Development.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holger/Documents/Git/spotfire-kanban/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248F3688-D6A1-D34A-848C-5AB150B69EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5885EFC8-B6D1-A54D-A48D-FE46CC299943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{61C5E4BF-0539-FB4F-8BC4-43AAC494A18A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="36">
   <si>
     <t>Task</t>
   </si>
@@ -118,6 +118,21 @@
   </si>
   <si>
     <t>As stakeholder I have access to the recent deployments from my investment view</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>asterix</t>
+  </si>
+  <si>
+    <t>trophy</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>wrong</t>
   </si>
 </sst>
 </file>
@@ -180,13 +195,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F92EC8DB-2A62-C246-B6D8-85B805D1DB14}" name="Tabelle1" displayName="Tabelle1" ref="A1:D19" totalsRowShown="0">
-  <autoFilter ref="A1:D19" xr:uid="{F92EC8DB-2A62-C246-B6D8-85B805D1DB14}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F92EC8DB-2A62-C246-B6D8-85B805D1DB14}" name="Tabelle1" displayName="Tabelle1" ref="A1:E19" totalsRowShown="0">
+  <autoFilter ref="A1:E19" xr:uid="{F92EC8DB-2A62-C246-B6D8-85B805D1DB14}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{516A9C67-3689-5141-A600-B3265FD734AB}" name="Task" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{F68AEB48-91F6-4F47-AE4C-A8444F5191BB}" name="Status"/>
     <tableColumn id="3" xr3:uid="{2D9D57E1-D432-1640-965F-7504A5116577}" name="Status Group"/>
     <tableColumn id="4" xr3:uid="{AC380817-2942-9347-B7B2-8A59F0231CD7}" name="Category"/>
+    <tableColumn id="5" xr3:uid="{ACDEB191-9920-FF43-ADAF-C0EFEA5B9C02}" name="Icon"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -489,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366F3820-3871-9545-9170-FE90875103A3}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +518,7 @@
     <col min="3" max="3" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +531,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -527,7 +546,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -541,7 +560,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -552,7 +571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -565,8 +584,11 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -577,7 +599,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -588,7 +610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -602,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -613,7 +635,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
@@ -624,7 +646,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -635,7 +657,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -645,8 +667,11 @@
       <c r="C12" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>23</v>
       </c>
@@ -659,8 +684,11 @@
       <c r="D13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -673,8 +701,11 @@
       <c r="D14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -685,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
Typo in asterisk vs asterix
</commit_message>
<xml_diff>
--- a/examples/Team Board for Product Development.xlsx
+++ b/examples/Team Board for Product Development.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/holger/Documents/Git/spotfire-kanban/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5885EFC8-B6D1-A54D-A48D-FE46CC299943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F923DD-4789-E646-92AF-D06BD9CEC2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{61C5E4BF-0539-FB4F-8BC4-43AAC494A18A}"/>
   </bookViews>
@@ -123,16 +123,16 @@
     <t>Icon</t>
   </si>
   <si>
-    <t>asterix</t>
-  </si>
-  <si>
     <t>trophy</t>
   </si>
   <si>
     <t>comments</t>
   </si>
   <si>
-    <t>wrong</t>
+    <t>asterisk</t>
+  </si>
+  <si>
+    <t>_test_</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -668,7 +668,7 @@
         <v>15</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -685,7 +685,7 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">

</xml_diff>